<commit_message>
Updated Task dated 07/03/2018
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="495" windowWidth="19815" windowHeight="7110" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="19815" windowHeight="7110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rajesh.E" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="132">
   <si>
     <t>S.no</t>
   </si>
@@ -409,6 +409,18 @@
   </si>
   <si>
     <t>Prepared for review in college</t>
+  </si>
+  <si>
+    <t>02-28-2018</t>
+  </si>
+  <si>
+    <t>8.30-12.15</t>
+  </si>
+  <si>
+    <t>EXAMS</t>
+  </si>
+  <si>
+    <t>12.15-4.30</t>
   </si>
 </sst>
 </file>
@@ -584,7 +596,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,6 +666,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -965,7 +980,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54:E54"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1658,15 +1673,1831 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="32">
+        <v>43103</v>
+      </c>
+      <c r="E56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="32">
+        <v>43134</v>
+      </c>
+      <c r="E57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="22">
+        <v>43162</v>
+      </c>
+      <c r="E58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="22">
+        <v>43193</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D61" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D62" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="22"/>
+      <c r="D63" t="s">
+        <v>131</v>
+      </c>
+      <c r="E63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1002"/>
+  <sheetViews>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="26" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="17">
+        <v>43132</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="17">
+        <v>43160</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="17">
+        <v>43191</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="17">
+        <v>43313</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="17">
+        <v>43344</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="17">
+        <v>43374</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="17">
+        <v>43405</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="21">
+        <v>43102</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="17">
+        <v>43133</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="17">
+        <v>43161</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="17">
+        <v>43192</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="17">
+        <v>43222</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="17">
+        <v>43253</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="22">
+        <v>43283</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="22">
+        <v>43314</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="22">
+        <v>43345</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="22">
+        <v>43375</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="22">
+        <v>43406</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="22">
+        <v>43436</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="32">
+        <v>43103</v>
+      </c>
+      <c r="E54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="32">
+        <v>43134</v>
+      </c>
+      <c r="E55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="22">
+        <v>43162</v>
+      </c>
+      <c r="E56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="22">
+        <v>43193</v>
+      </c>
+      <c r="E57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D58" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="22"/>
+      <c r="D61" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D62" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>131</v>
+      </c>
+      <c r="E63" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2604,1642 +4435,8 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1000"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:E52"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="26" width="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="17">
-        <v>43132</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="17">
-        <v>43160</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="17">
-        <v>43191</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="17">
-        <v>43313</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="17">
-        <v>43344</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="17">
-        <v>43374</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="17">
-        <v>43405</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="21">
-        <v>43102</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="17">
-        <v>43133</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="17">
-        <v>43161</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="17">
-        <v>43192</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="17">
-        <v>43222</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="17">
-        <v>43253</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="22">
-        <v>43283</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="22">
-        <v>43314</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="22">
-        <v>43345</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="22">
-        <v>43375</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="22">
-        <v>43406</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="22">
-        <v>43436</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E51" t="s">
-        <v>124</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5589,8 +5786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6194,22 +6391,112 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C49" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="32">
+        <v>43103</v>
+      </c>
+      <c r="E50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="32">
+        <v>43134</v>
+      </c>
+      <c r="E51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="22">
+        <v>43162</v>
+      </c>
+      <c r="E52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="22">
+        <v>43193</v>
+      </c>
+      <c r="E53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C54" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D54" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C55" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C56" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D56" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C57" s="22"/>
+      <c r="D57" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C58" s="22">
+        <v>43223</v>
+      </c>
+      <c r="D58" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated task dated 14/03/2018
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="133">
   <si>
     <t>S.no</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>12.15-4.30</t>
+  </si>
+  <si>
+    <t>PLACEMENT</t>
   </si>
 </sst>
 </file>
@@ -661,14 +664,14 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -979,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68:D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1682,7 +1685,7 @@
       </c>
     </row>
     <row r="56" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="32">
+      <c r="C56" s="30">
         <v>43103</v>
       </c>
       <c r="E56" t="s">
@@ -1690,7 +1693,7 @@
       </c>
     </row>
     <row r="57" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="32">
+      <c r="C57" s="30">
         <v>43134</v>
       </c>
       <c r="E57" t="s">
@@ -1737,7 +1740,7 @@
     </row>
     <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="22">
-        <v>43223</v>
+        <v>43254</v>
       </c>
       <c r="D62" t="s">
         <v>129</v>
@@ -1757,7 +1760,7 @@
     </row>
     <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" s="22">
-        <v>43223</v>
+        <v>43284</v>
       </c>
       <c r="D64" t="s">
         <v>129</v>
@@ -1766,7 +1769,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D65" t="s">
         <v>131</v>
       </c>
@@ -1774,21 +1777,55 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="4:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="22">
+        <v>43315</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E66" t="s">
+        <v>116</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="22">
+        <v>43346</v>
+      </c>
+      <c r="D67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="22">
+        <v>43376</v>
+      </c>
+      <c r="D68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="22">
+        <v>43407</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2718,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3406,7 +3443,7 @@
       </c>
     </row>
     <row r="54" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="32">
+      <c r="C54" s="30">
         <v>43103</v>
       </c>
       <c r="E54" t="s">
@@ -3414,7 +3451,7 @@
       </c>
     </row>
     <row r="55" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="32">
+      <c r="C55" s="30">
         <v>43134</v>
       </c>
       <c r="E55" t="s">
@@ -3461,7 +3498,7 @@
     </row>
     <row r="60" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C60" s="22">
-        <v>43223</v>
+        <v>43254</v>
       </c>
       <c r="D60" t="s">
         <v>129</v>
@@ -3481,7 +3518,7 @@
     </row>
     <row r="62" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="22">
-        <v>43223</v>
+        <v>43284</v>
       </c>
       <c r="D62" t="s">
         <v>129</v>
@@ -3498,23 +3535,57 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="22">
+        <v>43315</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="22">
+        <v>43346</v>
+      </c>
+      <c r="D65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="22">
+        <v>43376</v>
+      </c>
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="22">
+        <v>43407</v>
+      </c>
+      <c r="D67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5786,8 +5857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5954,7 +6025,7 @@
       <c r="D11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="31" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -5966,7 +6037,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6391,7 +6462,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C49" s="28" t="s">
         <v>128</v>
       </c>
@@ -6399,23 +6470,23 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C50" s="32">
+    <row r="50" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="30">
         <v>43103</v>
       </c>
       <c r="E50" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C51" s="32">
+    <row r="51" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="30">
         <v>43134</v>
       </c>
       <c r="E51" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C52" s="22">
         <v>43162</v>
       </c>
@@ -6423,7 +6494,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C53" s="22">
         <v>43193</v>
       </c>
@@ -6431,7 +6502,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="22">
         <v>43223</v>
       </c>
@@ -6442,7 +6513,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="22">
         <v>43223</v>
       </c>
@@ -6453,9 +6524,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="22">
-        <v>43223</v>
+        <v>43254</v>
       </c>
       <c r="D56" t="s">
         <v>129</v>
@@ -6464,7 +6535,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="22"/>
       <c r="D57" t="s">
         <v>131</v>
@@ -6473,9 +6544,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="22">
-        <v>43223</v>
+        <v>43284</v>
       </c>
       <c r="D58" t="s">
         <v>129</v>
@@ -6484,7 +6555,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
         <v>131</v>
       </c>
@@ -6492,11 +6563,45 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="3:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="22">
+        <v>43315</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E60" t="s">
+        <v>116</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C61" s="22">
+        <v>43346</v>
+      </c>
+      <c r="D61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C62" s="22">
+        <v>43376</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C63" s="22">
+        <v>43407</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated task dated 20/03/2018
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="495" windowWidth="19815" windowHeight="7110" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="19815" windowHeight="7110"/>
   </bookViews>
   <sheets>
     <sheet name="Rajesh.E" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="146">
   <si>
     <t>S.no</t>
   </si>
@@ -424,6 +424,45 @@
   </si>
   <si>
     <t>PLACEMENT</t>
+  </si>
+  <si>
+    <t>03-13-2018</t>
+  </si>
+  <si>
+    <t>03-14-2018</t>
+  </si>
+  <si>
+    <t>9.00-4.00</t>
+  </si>
+  <si>
+    <t>Worked with the database</t>
+  </si>
+  <si>
+    <t>Worked with the PDF  to scrape multiple files</t>
+  </si>
+  <si>
+    <t>03-15-2018</t>
+  </si>
+  <si>
+    <t>03-16-2018</t>
+  </si>
+  <si>
+    <t>03-17-2018</t>
+  </si>
+  <si>
+    <t>03-18-2018</t>
+  </si>
+  <si>
+    <t>03-19-2018</t>
+  </si>
+  <si>
+    <t>checked the database flow</t>
+  </si>
+  <si>
+    <t>Integrated the workflow</t>
+  </si>
+  <si>
+    <t>Checked the workflow of the module</t>
   </si>
 </sst>
 </file>
@@ -599,7 +638,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,6 +712,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -982,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68:D69"/>
+    <sheetView tabSelected="1" topLeftCell="B57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1815,14 +1856,106 @@
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="22">
+        <v>43437</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E71" t="s">
+        <v>136</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72" t="s">
+        <v>136</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D73" t="s">
+        <v>135</v>
+      </c>
+      <c r="E73" t="s">
+        <v>136</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" t="s">
+        <v>135</v>
+      </c>
+      <c r="E74" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>140</v>
+      </c>
+      <c r="D75" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>141</v>
+      </c>
+      <c r="D76" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>142</v>
+      </c>
+      <c r="D77" t="s">
+        <v>135</v>
+      </c>
+      <c r="E77" t="s">
+        <v>144</v>
+      </c>
+      <c r="F77" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="78" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="80" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2755,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66:D67"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3549,7 +3682,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C65" s="22">
         <v>43346</v>
       </c>
@@ -3557,7 +3690,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C66" s="22">
         <v>43376</v>
       </c>
@@ -3565,7 +3698,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="67" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" s="22">
         <v>43407</v>
       </c>
@@ -3573,19 +3706,99 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="22">
+        <v>43437</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" t="s">
+        <v>135</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5857,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62:D63"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6601,23 +6814,109 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="22">
+        <v>43437</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" t="s">
+        <v>116</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E65" t="s">
+        <v>116</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" t="s">
+        <v>116</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" t="s">
+        <v>116</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" t="s">
+        <v>145</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="3:6" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="81" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="82" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="83" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>